<commit_message>
Final push with the report
</commit_message>
<xml_diff>
--- a/Semester4GameDevProject/Documentation/Project_TimeActivity.xlsx
+++ b/Semester4GameDevProject/Documentation/Project_TimeActivity.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -96,12 +96,6 @@
     <t>Designing</t>
   </si>
   <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Created a test player character, player animations, sword and floor. Forgot to make elbows and knees on the character models</t>
   </si>
   <si>
@@ -241,6 +235,15 @@
   </si>
   <si>
     <t>Worked on the animator for monsters/enemies and refactored the way the loot works</t>
+  </si>
+  <si>
+    <t>Created weapons and potions. Worked on the town and start are. Added lights. Refactored the passages to work better.</t>
+  </si>
+  <si>
+    <t>Worked on the story of the game and started to add NPC's with quests that are tied to the story.</t>
+  </si>
+  <si>
+    <t>Started to work on the collect quest so it count properly on the items collected and made the quest giver remove th item from the players list(not UI)</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -724,6 +727,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -968,22 +974,20 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
+                <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
-              </a:rPr>
+              <a:rPr lang="en-US"/>
               <a:t>Time Used on  Project</a:t>
             </a:r>
           </a:p>
@@ -1010,11 +1014,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
+              <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -1030,10 +1037,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.1208759161515066E-2"/>
-          <c:y val="0.36579555006604564"/>
+          <c:x val="1.9879364531078685E-2"/>
+          <c:y val="7.3112476794059272E-2"/>
           <c:w val="0.84022933030807034"/>
-          <c:h val="0.44821985487108229"/>
+          <c:h val="0.74090263107355481"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1041,22 +1048,22 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Activity Tracker'!$A$3</c:f>
+              <c:f>'Activity Tracker'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Planning</c:v>
+                  <c:v>Unity</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1073,13 +1080,18 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1099,6 +1111,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1130,36 +1143,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Activity Tracker'!$B$5</c:f>
+              <c:f>'Activity Tracker'!$B$7:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:formatCode>#,#00</c:formatCode>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>105.16666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Activity Tracker'!$A$7</c:f>
+              <c:f>'Activity Tracker'!$A$11:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Unity</c:v>
+                  <c:v>Designing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent3"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1176,13 +1187,18 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="bg1"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1202,6 +1218,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1233,248 +1250,76 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Activity Tracker'!$B$9</c:f>
+              <c:f>'Activity Tracker'!$B$11:$B$12</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5690</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Activity Tracker'!$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Designing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Activity Tracker'!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Project</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Activity Tracker'!$B$13</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>750</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Activity Tracker'!$A$15:$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Testing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="bg1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Activity Tracker'!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Project</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Activity Tracker'!$B$17:$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>#,#00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="40"/>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-1946393840"/>
-        <c:axId val="-1946390032"/>
+        <c:axId val="1690742464"/>
+        <c:axId val="1690745728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1946393840"/>
+        <c:axId val="1690742464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1946390032"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1690745728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1482,7 +1327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1946390032"/>
+        <c:axId val="1690745728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1502,7 +1347,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,#00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1518,7 +1363,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1533,7 +1378,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1946393840"/>
+        <c:crossAx val="1690742464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,7 +1391,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.43218072815673714"/>
+          <c:y val="0.74085269829076239"/>
+          <c:w val="0.1196864001172336"/>
+          <c:h val="0.13719608219704246"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1581,9 +1436,16 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1593,7 +1455,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -2187,7 +2049,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="List" displayName="List" ref="E5:J51" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="List" displayName="List" ref="E5:J54" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Subject" dataDxfId="4"/>
@@ -2496,10 +2358,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2550,20 +2412,15 @@
       </c>
       <c r="N2" s="47">
         <f>SUM(B17,B13,B9,B5)</f>
-        <v>6440</v>
+        <v>7060</v>
       </c>
       <c r="O2" s="49" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="39">
-        <f>SUMIF(List[Subject],Category1,List[Minutes])/60</f>
-        <v>0</v>
-      </c>
+      <c r="A3" s="41"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="13"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -2578,9 +2435,7 @@
     <row r="4" spans="1:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="41"/>
       <c r="B4" s="39"/>
-      <c r="C4" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="C4" s="10"/>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4" s="23"/>
@@ -2589,7 +2444,7 @@
       </c>
       <c r="N4" s="52">
         <f>SUM(N2)/60</f>
-        <v>107.33333333333333</v>
+        <v>117.66666666666667</v>
       </c>
       <c r="O4" s="49" t="s">
         <v>9</v>
@@ -2597,13 +2452,8 @@
     </row>
     <row r="5" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="41"/>
-      <c r="B5" s="43">
-        <f>SUMIF(List[Subject],Category1,List[Minutes])</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="11"/>
       <c r="E5" s="21" t="s">
         <v>0</v>
       </c>
@@ -2646,23 +2496,23 @@
         <v>300</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="39">
+        <v>17</v>
+      </c>
+      <c r="B7" s="55">
         <f>SUMIF(List[Subject],Category2,List[Minutes])/60</f>
-        <v>94.833333333333329</v>
+        <v>105.16666666666667</v>
       </c>
       <c r="C7" s="15"/>
       <c r="E7" s="31">
         <v>43152</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="33">
         <v>0.4861111111111111</v>
@@ -2674,7 +2524,7 @@
         <v>40</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2687,7 +2537,7 @@
         <v>43152</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G8" s="33">
         <v>0.82638888888888884</v>
@@ -2699,14 +2549,14 @@
         <v>280</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="41"/>
       <c r="B9" s="43">
         <f>SUMIF(List[Subject],Category2,List[Minutes])</f>
-        <v>5690</v>
+        <v>6310</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>10</v>
@@ -2715,7 +2565,7 @@
         <v>43153</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G9" s="33">
         <v>0.58333333333333337</v>
@@ -2727,7 +2577,7 @@
         <v>80</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2738,7 +2588,7 @@
         <v>43153</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G10" s="33">
         <v>0.95486111111111116</v>
@@ -2750,7 +2600,7 @@
         <v>40</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2778,7 +2628,7 @@
         <v>130</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2803,7 +2653,7 @@
         <v>320</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2819,7 +2669,7 @@
         <v>43156</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G13" s="33">
         <v>0.54166666666666663</v>
@@ -2831,7 +2681,7 @@
         <v>140</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L13" s="6"/>
     </row>
@@ -2843,7 +2693,7 @@
         <v>43158</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G14" s="33">
         <v>0.875</v>
@@ -2855,25 +2705,20 @@
         <v>120</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:15" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="39">
-        <f>SUMIF(List[Subject],Category4,List[Minutes])/60</f>
-        <v>0</v>
-      </c>
+      <c r="A15" s="40"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="15"/>
       <c r="D15" s="5"/>
       <c r="E15" s="31">
         <v>43160</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G15" s="33">
         <v>0.77083333333333337</v>
@@ -2885,21 +2730,19 @@
         <v>210</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="41"/>
       <c r="B16" s="39"/>
-      <c r="C16" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="C16" s="10"/>
       <c r="D16" s="5"/>
       <c r="E16" s="31">
         <v>43161</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G16" s="33">
         <v>0.76388888888888884</v>
@@ -2911,24 +2754,19 @@
         <v>120</v>
       </c>
       <c r="J16" s="37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="41"/>
-      <c r="B17" s="43">
-        <f>SUMIF(List[Subject],Category4,List[Minutes])</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="5"/>
       <c r="E17" s="31">
         <v>43163</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G17" s="33">
         <v>0.625</v>
@@ -2940,7 +2778,7 @@
         <v>105</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2952,7 +2790,7 @@
         <v>43164</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G18" s="33">
         <v>0.93055555555555547</v>
@@ -2964,7 +2802,7 @@
         <v>40</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2973,7 +2811,7 @@
         <v>43165</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G19" s="33">
         <v>0.91666666666666663</v>
@@ -2985,7 +2823,7 @@
         <v>60</v>
       </c>
       <c r="J19" s="36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2994,7 +2832,7 @@
         <v>43166</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G20" s="33">
         <v>0.52777777777777779</v>
@@ -3006,7 +2844,7 @@
         <v>125</v>
       </c>
       <c r="J20" s="36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3015,7 +2853,7 @@
         <v>43168</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G21" s="33">
         <v>0.76041666666666663</v>
@@ -3027,7 +2865,7 @@
         <v>40</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3036,7 +2874,7 @@
         <v>43173</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G22" s="33">
         <v>0.91666666666666663</v>
@@ -3048,7 +2886,7 @@
         <v>60</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3056,7 +2894,7 @@
         <v>43174</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G23" s="33">
         <v>0.5</v>
@@ -3068,7 +2906,7 @@
         <v>210</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3076,7 +2914,7 @@
         <v>43176</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G24" s="33">
         <v>0.58333333333333337</v>
@@ -3088,7 +2926,7 @@
         <v>200</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3096,7 +2934,7 @@
         <v>43183</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G25" s="33">
         <v>0.42708333333333331</v>
@@ -3108,7 +2946,7 @@
         <v>120</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3116,7 +2954,7 @@
         <v>43184</v>
       </c>
       <c r="F26" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G26" s="33">
         <v>0.59375</v>
@@ -3128,7 +2966,7 @@
         <v>150</v>
       </c>
       <c r="J26" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3136,7 +2974,7 @@
         <v>43191</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G27" s="33">
         <v>0.4236111111111111</v>
@@ -3148,7 +2986,7 @@
         <v>180</v>
       </c>
       <c r="J27" s="36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3156,7 +2994,7 @@
         <v>43195</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G28" s="33">
         <v>0.50694444444444442</v>
@@ -3168,7 +3006,7 @@
         <v>120</v>
       </c>
       <c r="J28" s="36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3176,7 +3014,7 @@
         <v>43197</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G29" s="33">
         <v>0.45833333333333331</v>
@@ -3188,7 +3026,7 @@
         <v>180</v>
       </c>
       <c r="J29" s="36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3196,7 +3034,7 @@
         <v>43198</v>
       </c>
       <c r="F30" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G30" s="33">
         <v>0.39583333333333331</v>
@@ -3208,7 +3046,7 @@
         <v>120</v>
       </c>
       <c r="J30" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3216,7 +3054,7 @@
         <v>43200</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G31" s="33">
         <v>0.47916666666666669</v>
@@ -3228,7 +3066,7 @@
         <v>150</v>
       </c>
       <c r="J31" s="36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3236,7 +3074,7 @@
         <v>43204</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G32" s="33">
         <v>0.58333333333333337</v>
@@ -3248,7 +3086,7 @@
         <v>70</v>
       </c>
       <c r="J32" s="36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3256,7 +3094,7 @@
         <v>43209</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G33" s="33">
         <v>0.40277777777777773</v>
@@ -3268,7 +3106,7 @@
         <v>140</v>
       </c>
       <c r="J33" s="36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3276,7 +3114,7 @@
         <v>43210</v>
       </c>
       <c r="F34" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G34" s="33">
         <v>0.4236111111111111</v>
@@ -3288,7 +3126,7 @@
         <v>135</v>
       </c>
       <c r="J34" s="36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3296,7 +3134,7 @@
         <v>43217</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G35" s="33">
         <v>0.63194444444444442</v>
@@ -3308,7 +3146,7 @@
         <v>90</v>
       </c>
       <c r="J35" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3316,7 +3154,7 @@
         <v>43219</v>
       </c>
       <c r="F36" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G36" s="33">
         <v>0.47916666666666669</v>
@@ -3328,7 +3166,7 @@
         <v>80</v>
       </c>
       <c r="J36" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3336,7 +3174,7 @@
         <v>43222</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G37" s="33">
         <v>0.4375</v>
@@ -3348,7 +3186,7 @@
         <v>75</v>
       </c>
       <c r="J37" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3356,7 +3194,7 @@
         <v>43223</v>
       </c>
       <c r="F38" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G38" s="33">
         <v>0.4236111111111111</v>
@@ -3368,7 +3206,7 @@
         <v>150</v>
       </c>
       <c r="J38" s="36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3376,7 +3214,7 @@
         <v>43225</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G39" s="33">
         <v>0.41666666666666669</v>
@@ -3388,7 +3226,7 @@
         <v>285</v>
       </c>
       <c r="J39" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3396,7 +3234,7 @@
         <v>43226</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G40" s="33">
         <v>0.4201388888888889</v>
@@ -3408,7 +3246,7 @@
         <v>110</v>
       </c>
       <c r="J40" s="36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3416,7 +3254,7 @@
         <v>43226</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G41" s="33">
         <v>0.62847222222222221</v>
@@ -3428,7 +3266,7 @@
         <v>45</v>
       </c>
       <c r="J41" s="36" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3436,7 +3274,7 @@
         <v>43227</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G42" s="33">
         <v>0.46875</v>
@@ -3448,7 +3286,7 @@
         <v>100</v>
       </c>
       <c r="J42" s="36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3456,7 +3294,7 @@
         <v>43227</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G43" s="33">
         <v>0.59375</v>
@@ -3468,7 +3306,7 @@
         <v>75</v>
       </c>
       <c r="J43" s="36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3476,7 +3314,7 @@
         <v>43228</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G44" s="33">
         <v>0.55555555555555558</v>
@@ -3488,7 +3326,7 @@
         <v>185</v>
       </c>
       <c r="J44" s="36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3496,7 +3334,7 @@
         <v>43229</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G45" s="33">
         <v>0.45833333333333331</v>
@@ -3508,7 +3346,7 @@
         <v>230</v>
       </c>
       <c r="J45" s="36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3516,7 +3354,7 @@
         <v>43230</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G46" s="33">
         <v>0.36458333333333331</v>
@@ -3528,7 +3366,7 @@
         <v>155</v>
       </c>
       <c r="J46" s="36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3536,7 +3374,7 @@
         <v>43232</v>
       </c>
       <c r="F47" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G47" s="33">
         <v>0.44444444444444442</v>
@@ -3548,7 +3386,7 @@
         <v>150</v>
       </c>
       <c r="J47" s="36" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3556,7 +3394,7 @@
         <v>43233</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G48" s="33">
         <v>0.41666666666666669</v>
@@ -3568,7 +3406,7 @@
         <v>240</v>
       </c>
       <c r="J48" s="36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3576,7 +3414,7 @@
         <v>43235</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G49" s="33">
         <v>0.375</v>
@@ -3588,7 +3426,7 @@
         <v>300</v>
       </c>
       <c r="J49" s="36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3596,7 +3434,7 @@
         <v>43236</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G50" s="33">
         <v>0.3576388888888889</v>
@@ -3608,7 +3446,7 @@
         <v>120</v>
       </c>
       <c r="J50" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3616,7 +3454,7 @@
         <v>43236</v>
       </c>
       <c r="F51" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G51" s="33">
         <v>0.56597222222222221</v>
@@ -3628,7 +3466,67 @@
         <v>65</v>
       </c>
       <c r="J51" s="36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E52" s="31">
+        <v>43237</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" s="33">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="H52" s="34">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I52" s="35">
+        <v>240</v>
+      </c>
+      <c r="J52" s="36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E53" s="31">
+        <v>43238</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G53" s="33">
+        <v>0.375</v>
+      </c>
+      <c r="H53" s="34">
+        <v>0.15625</v>
+      </c>
+      <c r="I53" s="35">
+        <v>225</v>
+      </c>
+      <c r="J53" s="36" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="5:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E54" s="31">
+        <v>43239</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" s="33">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="H54" s="34">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="I54" s="35">
+        <v>155</v>
+      </c>
+      <c r="J54" s="36" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3720,11 +3618,11 @@
     <row r="4" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" t="str">
         <f>TRIM(Category1)</f>
-        <v>Planning</v>
-      </c>
-      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="C4">
         <f>Category1Unit</f>
-        <v>Hours</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>